<commit_message>
added teamFlags and cleaned up CONTROL patch
</commit_message>
<xml_diff>
--- a/_assets/_TEAMS/muster-teams.xlsx
+++ b/_assets/_TEAMS/muster-teams.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t xml:space="preserve">FLL Europafinale</t>
   </si>
@@ -44,6 +44,24 @@
   </si>
   <si>
     <t xml:space="preserve">05 – Bhof-Bots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">france</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03 – Robocops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">belgium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04 – Schokis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSOG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">switzerland</t>
   </si>
 </sst>
 </file>
@@ -163,10 +181,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -226,7 +244,55 @@
         <v>5</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>